<commit_message>
updated 'basic stats' and renamed xmind files
</commit_message>
<xml_diff>
--- a/data/basic stats.xlsx
+++ b/data/basic stats.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shanekercheval/OneDrive/stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shanekercheval/OneDrive/gitrepos/tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1228,7 +1228,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1375,11 +1374,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2131913744"/>
-        <c:axId val="-2131908592"/>
+        <c:axId val="2145148000"/>
+        <c:axId val="2145155984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131913744"/>
+        <c:axId val="2145148000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1410,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1478,7 +1476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131908592"/>
+        <c:crossAx val="2145155984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131908592"/>
+        <c:axId val="2145155984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1516,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1579,7 +1576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131913744"/>
+        <c:crossAx val="2145148000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1593,7 +1590,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2504,7 +2500,7 @@
   <dimension ref="A1:K315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>